<commit_message>
Programa 1 casi listo
Fatla la pregunta 7
</commit_message>
<xml_diff>
--- a/Tabla.xlsx
+++ b/Tabla.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Usuarios\meramirez\Desktop\TEC\CURSOS\2016\II Semestre\ALC\Tarea #1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liza\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12190" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2011-2012" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -272,7 +272,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -364,6 +364,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -399,6 +416,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -553,16 +587,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.08984375" customWidth="1"/>
+    <col min="3" max="3" width="5.90625" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="5" width="5.90625" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -591,7 +630,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -620,7 +659,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -649,7 +688,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+    <row r="4" spans="1:9" ht="15" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
@@ -678,7 +717,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+    <row r="5" spans="1:9" ht="15" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
@@ -707,7 +746,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -736,7 +775,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+    <row r="7" spans="1:9" ht="15" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -765,7 +804,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1">
+    <row r="8" spans="1:9" ht="15" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -794,7 +833,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+    <row r="9" spans="1:9" ht="15" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -823,7 +862,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+    <row r="10" spans="1:9" ht="15" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
@@ -852,7 +891,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -881,7 +920,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+    <row r="12" spans="1:9" ht="15" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
@@ -910,7 +949,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+    <row r="13" spans="1:9" ht="15" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
@@ -939,7 +978,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+    <row r="14" spans="1:9" ht="15" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -968,7 +1007,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1">
+    <row r="15" spans="1:9" ht="15" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>22</v>
       </c>
@@ -997,7 +1036,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
+    <row r="16" spans="1:9" ht="15" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>23</v>
       </c>
@@ -1026,7 +1065,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+    <row r="17" spans="1:9" ht="15" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>24</v>
       </c>
@@ -1055,7 +1094,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
+    <row r="18" spans="1:9" ht="15" thickBot="1">
       <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
@@ -1084,7 +1123,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+    <row r="19" spans="1:9" ht="15" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>26</v>
       </c>
@@ -1113,7 +1152,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
+    <row r="20" spans="1:9" ht="15" thickBot="1">
       <c r="A20" s="6" t="s">
         <v>27</v>
       </c>
@@ -1192,15 +1231,15 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -1229,7 +1268,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1258,7 +1297,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -1287,7 +1326,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+    <row r="4" spans="1:9" ht="15" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -1316,7 +1355,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+    <row r="5" spans="1:9" ht="15" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
@@ -1345,7 +1384,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -1374,7 +1413,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+    <row r="7" spans="1:9" ht="15" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1403,7 +1442,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1">
+    <row r="8" spans="1:9" ht="15" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -1432,7 +1471,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+    <row r="9" spans="1:9" ht="15" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1461,7 +1500,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+    <row r="10" spans="1:9" ht="15" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
@@ -1490,7 +1529,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -1519,7 +1558,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+    <row r="12" spans="1:9" ht="15" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
@@ -1548,7 +1587,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+    <row r="13" spans="1:9" ht="15" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
@@ -1577,7 +1616,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+    <row r="14" spans="1:9" ht="15" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
@@ -1606,7 +1645,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1">
+    <row r="15" spans="1:9" ht="15" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>30</v>
       </c>
@@ -1635,7 +1674,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
+    <row r="16" spans="1:9" ht="15" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
@@ -1664,7 +1703,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+    <row r="17" spans="1:9" ht="15" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
@@ -1693,7 +1732,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
+    <row r="18" spans="1:9" ht="15" thickBot="1">
       <c r="A18" s="6" t="s">
         <v>31</v>
       </c>
@@ -1722,7 +1761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+    <row r="19" spans="1:9" ht="15" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
@@ -1751,7 +1790,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
+    <row r="20" spans="1:9" ht="15" thickBot="1">
       <c r="A20" s="6" t="s">
         <v>32</v>
       </c>
@@ -1832,12 +1871,12 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
@@ -1866,7 +1905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
@@ -1895,7 +1934,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -1924,7 +1963,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+    <row r="4" spans="1:9" ht="15" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -1953,7 +1992,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+    <row r="5" spans="1:9" ht="15" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -1982,7 +2021,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
@@ -2011,7 +2050,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+    <row r="7" spans="1:9" ht="15" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
@@ -2040,7 +2079,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1">
+    <row r="8" spans="1:9" ht="15" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -2069,7 +2108,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+    <row r="9" spans="1:9" ht="15" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -2098,7 +2137,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+    <row r="10" spans="1:9" ht="15" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>31</v>
       </c>
@@ -2127,7 +2166,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
@@ -2156,7 +2195,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+    <row r="12" spans="1:9" ht="15" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -2185,7 +2224,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+    <row r="13" spans="1:9" ht="15" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
@@ -2214,7 +2253,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+    <row r="14" spans="1:9" ht="15" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
@@ -2243,7 +2282,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1">
+    <row r="15" spans="1:9" ht="15" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>22</v>
       </c>
@@ -2272,7 +2311,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
+    <row r="16" spans="1:9" ht="15" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
@@ -2301,7 +2340,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+    <row r="17" spans="1:9" ht="15" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>34</v>
       </c>
@@ -2330,7 +2369,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
+    <row r="18" spans="1:9" ht="15" thickBot="1">
       <c r="A18" s="6" t="s">
         <v>35</v>
       </c>
@@ -2359,7 +2398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+    <row r="19" spans="1:9" ht="15" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
@@ -2388,7 +2427,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
+    <row r="20" spans="1:9" ht="15" thickBot="1">
       <c r="A20" s="6" t="s">
         <v>30</v>
       </c>
@@ -2469,12 +2508,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
@@ -2503,7 +2542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -2532,7 +2571,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -2561,7 +2600,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+    <row r="4" spans="1:9" ht="15" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -2590,7 +2629,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+    <row r="5" spans="1:9" ht="15" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -2619,7 +2658,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
@@ -2648,7 +2687,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+    <row r="7" spans="1:9" ht="15" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
@@ -2677,7 +2716,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1">
+    <row r="8" spans="1:9" ht="15" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -2706,7 +2745,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+    <row r="9" spans="1:9" ht="15" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
@@ -2735,7 +2774,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+    <row r="10" spans="1:9" ht="15" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -2764,7 +2803,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
@@ -2793,7 +2832,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+    <row r="12" spans="1:9" ht="15" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>23</v>
       </c>
@@ -2822,7 +2861,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+    <row r="13" spans="1:9" ht="15" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
@@ -2851,7 +2890,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+    <row r="14" spans="1:9" ht="15" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>34</v>
       </c>
@@ -2880,7 +2919,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1">
+    <row r="15" spans="1:9" ht="15" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
@@ -2909,7 +2948,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
+    <row r="16" spans="1:9" ht="15" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>19</v>
       </c>
@@ -2938,7 +2977,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+    <row r="17" spans="1:9" ht="15" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
@@ -2967,7 +3006,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
+    <row r="18" spans="1:9" ht="15" thickBot="1">
       <c r="A18" s="6" t="s">
         <v>25</v>
       </c>
@@ -2996,7 +3035,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+    <row r="19" spans="1:9" ht="15" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>37</v>
       </c>
@@ -3025,7 +3064,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
+    <row r="20" spans="1:9" ht="15" thickBot="1">
       <c r="A20" s="6" t="s">
         <v>35</v>
       </c>
@@ -3102,16 +3141,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+    <row r="1" spans="1:9" ht="15" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>39</v>
       </c>
@@ -3140,7 +3179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -3169,7 +3208,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1">
+    <row r="3" spans="1:9" ht="15" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -3195,10 +3234,10 @@
         <v>76</v>
       </c>
       <c r="I3" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
@@ -3227,7 +3266,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1">
+    <row r="5" spans="1:9" ht="15" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -3256,7 +3295,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1">
+    <row r="6" spans="1:9" ht="15" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -3285,7 +3324,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+    <row r="7" spans="1:9" ht="15" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -3314,7 +3353,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1">
+    <row r="8" spans="1:9" ht="15" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -3343,7 +3382,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1">
+    <row r="9" spans="1:9" ht="15" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
@@ -3372,7 +3411,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1">
+    <row r="10" spans="1:9" ht="15" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
@@ -3401,7 +3440,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1">
+    <row r="11" spans="1:9" ht="15" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -3430,7 +3469,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+    <row r="12" spans="1:9" ht="15" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>40</v>
       </c>
@@ -3459,7 +3498,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1">
+    <row r="13" spans="1:9" ht="15" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
@@ -3488,7 +3527,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1">
+    <row r="14" spans="1:9" ht="15" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
@@ -3517,7 +3556,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1">
+    <row r="15" spans="1:9" ht="15" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -3546,7 +3585,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1">
+    <row r="16" spans="1:9" ht="15" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
@@ -3575,7 +3614,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+    <row r="17" spans="1:9" ht="15" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>25</v>
       </c>
@@ -3604,7 +3643,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1">
+    <row r="18" spans="1:9" ht="15" thickBot="1">
       <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
@@ -3633,7 +3672,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+    <row r="19" spans="1:9" ht="15" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
@@ -3662,7 +3701,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
+    <row r="20" spans="1:9" ht="15" thickBot="1">
       <c r="A20" s="6" t="s">
         <v>19</v>
       </c>

</xml_diff>